<commit_message>
fixed Senate raw data error, resolved slice max vs. filter issue
</commit_message>
<xml_diff>
--- a/data/Election Validation/Final Sets - Clean Fixed/Senate_0622_clean_fixed.xlsx
+++ b/data/Election Validation/Final Sets - Clean Fixed/Senate_0622_clean_fixed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdpruett/Desktop/PPRG/PPRG_R_Directory/Election Validation/Final Sets - Clean Fixed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdpruett/Desktop/CES Accuracy Analysis/data/Election Validation/Final Sets - Clean Fixed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8533BACE-DBFC-004D-8CD8-87B148C60411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70E2EFB-9FB2-E141-8AAA-A1FFB6645CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4446,9 +4446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1228" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1249" sqref="Q1249"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1398" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1421" sqref="M1421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -72957,7 +72957,7 @@
         <v>278503</v>
       </c>
       <c r="N1420" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="O1420">
         <v>2</v>
@@ -73007,7 +73007,7 @@
         <v>278503</v>
       </c>
       <c r="N1421" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O1421">
         <v>1</v>

</xml_diff>